<commit_message>
Create all control_db tables
</commit_message>
<xml_diff>
--- a/documentation/Architecture.xlsx
+++ b/documentation/Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\ADF-Metada-Driven\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26071BA3-B24E-4E70-B0C5-D56A809D742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CFC656-AC4B-4ADD-ACAB-CD5169B61385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5BD82074-C620-4ADE-AEBD-3CA95536FC80}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>Template csv / ctl.file</t>
   </si>
   <si>
-    <t>ctl.file</t>
-  </si>
-  <si>
     <t>vchar</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>status_type</t>
+  </si>
+  <si>
+    <t>ctl.file_template</t>
   </si>
 </sst>
 </file>
@@ -2224,12 +2224,12 @@
   <dimension ref="B3:O33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2286,13 +2286,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
@@ -2318,13 +2318,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>22</v>
@@ -2350,7 +2350,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -2364,7 +2364,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -2372,13 +2372,13 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -2386,13 +2386,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
         <v>24</v>
@@ -2403,7 +2403,7 @@
         <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>21</v>
@@ -2421,13 +2421,13 @@
         <v>11</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -2438,10 +2438,10 @@
         <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>22</v>
@@ -2473,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -2489,7 +2489,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -2521,12 +2521,12 @@
         <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>26</v>
@@ -2534,10 +2534,10 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -2553,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -2594,7 +2594,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>26</v>
@@ -2602,18 +2602,18 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Architecture Add table_name.sql
</commit_message>
<xml_diff>
--- a/documentation/Architecture.xlsx
+++ b/documentation/Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\ADF-Metada-Driven\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CFC656-AC4B-4ADD-ACAB-CD5169B61385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3B9E0-1057-495D-AFB6-89F77412E11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5BD82074-C620-4ADE-AEBD-3CA95536FC80}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
   <si>
     <t>ctl.process</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t>ctl.file_template</t>
+  </si>
+  <si>
+    <t>ctl.table_name</t>
+  </si>
+  <si>
+    <t>table_name_id</t>
+  </si>
+  <si>
+    <t>Ingestion Table</t>
+  </si>
+  <si>
+    <t>Succeed</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -185,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +210,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,12 +253,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1906,6 +1942,411 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123436</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1245469" cy="311496"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="TextBox 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F873682-F6CB-4758-854C-C6853C0AAEDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733036" y="2814637"/>
+          <a:ext cx="1245469" cy="311496"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1400"/>
+            <a:t>CSV_Template</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1032334" cy="256737"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="TextBox 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD10030-DB99-496D-BE59-6E697B647ED5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="3181350"/>
+          <a:ext cx="1032334" cy="256737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1050"/>
+            <a:t>LS_Azure_ADLS</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1050" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1117229" cy="256737"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="TextBox 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21BCF70F-405B-4A60-B962-3C00FB490722}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="3505200"/>
+          <a:ext cx="1117229" cy="256737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1050"/>
+            <a:t>DS_ADLS_Source</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1050" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>532372</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="481542" cy="311496"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37254A17-EA13-42EE-917A-EB288A5B8D56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2970772" y="2805112"/>
+          <a:ext cx="481542" cy="311496"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1400"/>
+            <a:t>ADF</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>149705</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>103360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>532372</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>112885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{578F027A-4550-4774-956D-6E4B440A8656}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="36" idx="3"/>
+          <a:endCxn id="40" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1978505" y="2960860"/>
+          <a:ext cx="992267" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>404314</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>184323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>298311</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>103360</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Connector: Elbow 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E58FD5EC-62CA-46D1-B38E-1470263BE876}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="3"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3452314" y="2470323"/>
+          <a:ext cx="2941997" cy="490537"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Connector: Elbow 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F503A89-9401-4A98-A91C-4DC147674A56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2571751" y="1057275"/>
+          <a:ext cx="1704975" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 31565"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2209,7 +2650,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,403 +2662,493 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4D0F2E-3D71-4F93-8099-22CE3EC0826B}">
-  <dimension ref="B3:O33"/>
+  <dimension ref="B2:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="F12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="G12" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="3">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="F14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="F23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="F25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="F26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="F28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>